<commit_message>
mise en page des titres
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -1,27 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CVM\2014_2_Automne\A11\Documents\03 Microsoft Excel\Exercice02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF422200-DE73-48A5-994C-8E26E721F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22110" windowHeight="9285"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultat attendu" sheetId="1" r:id="rId1"/>
-    <sheet name="Données brutes" sheetId="2" r:id="rId2"/>
-    <sheet name="Objectifs" sheetId="3" r:id="rId3"/>
+    <sheet name="Résultat obtenu" sheetId="5" r:id="rId2"/>
+    <sheet name="Données brutes" sheetId="2" r:id="rId3"/>
+    <sheet name="Objectifs" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
   <si>
     <t>Compagnie X</t>
   </si>
@@ -134,13 +149,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +303,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +379,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -476,12 +505,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -502,11 +542,11 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
@@ -522,11 +562,11 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
@@ -560,10 +600,10 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -580,10 +620,10 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -637,7 +677,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -649,7 +689,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -658,7 +698,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -669,20 +709,20 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -692,19 +732,19 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -712,10 +752,10 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -724,7 +764,7 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -741,6 +781,15 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -842,6 +891,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -877,6 +943,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1052,26 +1135,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS50" sqref="AS50"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="11.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="11.5703125" style="3"/>
+    <col min="1" max="1" width="1.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.26953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="11.1796875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="1.7265625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,8 +1163,8 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="75" t="s">
         <v>18</v>
       </c>
@@ -1090,14 +1173,14 @@
       <c r="E4" s="75"/>
       <c r="F4" s="75"/>
     </row>
-    <row r="5" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>19</v>
@@ -1108,7 +1191,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14" t="s">
@@ -1117,7 +1200,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
@@ -1126,7 +1209,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
@@ -1135,8 +1218,8 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:10" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +1236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="11.5" x14ac:dyDescent="0.25">
       <c r="B12" s="20">
         <v>1</v>
       </c>
@@ -1172,7 +1255,7 @@
       </c>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="26">
         <v>2</v>
       </c>
@@ -1190,7 +1273,7 @@
         <v>999.98</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <v>3</v>
       </c>
@@ -1208,7 +1291,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="26">
         <v>4</v>
       </c>
@@ -1226,7 +1309,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="11.5" x14ac:dyDescent="0.25">
       <c r="B16" s="31">
         <v>5</v>
       </c>
@@ -1244,7 +1327,7 @@
       </c>
       <c r="J16" s="25"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="35">
         <v>6</v>
       </c>
@@ -1261,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="31">
         <v>7</v>
       </c>
@@ -1278,7 +1361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="35">
         <v>8</v>
       </c>
@@ -1295,7 +1378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="31">
         <v>9</v>
       </c>
@@ -1312,7 +1395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="39">
         <v>10</v>
       </c>
@@ -1329,8 +1412,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:6" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="43" t="s">
         <v>13</v>
       </c>
@@ -1340,10 +1423,10 @@
         <v>12099.98</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="46"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D25" s="47" t="s">
         <v>14</v>
       </c>
@@ -1352,7 +1435,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="50" t="s">
         <v>13</v>
       </c>
@@ -1362,10 +1445,10 @@
         <v>11599.98</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="53"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D28" s="54" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1460,7 @@
         <v>579.99900000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="57" t="s">
         <v>16</v>
       </c>
@@ -1389,10 +1472,10 @@
         <v>1157.0980050000001</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="53"/>
     </row>
-    <row r="31" spans="2:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D31" s="60" t="s">
         <v>17</v>
       </c>
@@ -1402,7 +1485,7 @@
         <v>13337.077004999999</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C+8qTaT+AjYg5X1U41RLreZfjPJvXO9YGqqTVDPRT4FUbAFcU6YpHGmJQDK+sylT6UupyQ3rsecUtR8wpbocAg==" saltValue="1TJbgLDI941YSuk2Qa1HqQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
@@ -1414,24 +1497,312 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6281C5BB-372A-4902-85E9-DFBE7E384DD1}">
   <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.5703125" style="63" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="63"/>
-    <col min="9" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="1.7265625" style="63" customWidth="1"/>
+    <col min="2" max="2" width="3.54296875" style="63" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" style="63" customWidth="1"/>
+    <col min="4" max="7" width="11.54296875" style="63" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="63"/>
+    <col min="9" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="78"/>
+      <c r="B2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+    </row>
+    <row r="6" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="63">
+        <v>1</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="63">
+        <v>15</v>
+      </c>
+      <c r="E12" s="64">
+        <v>45</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="63">
+        <v>2</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="63">
+        <v>2</v>
+      </c>
+      <c r="E13" s="64">
+        <v>499.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="63">
+        <v>3</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="63">
+        <v>5</v>
+      </c>
+      <c r="E14" s="64">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="63">
+        <v>4</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="63">
+        <v>120</v>
+      </c>
+      <c r="E15" s="64">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="63">
+        <v>5</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="63">
+        <v>6</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="63">
+        <v>7</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="63">
+        <v>8</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="63">
+        <v>9</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="63">
+        <v>10</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="64">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="63">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="63">
+        <v>9.9750000000000005E-2</v>
+      </c>
+      <c r="F29" s="64"/>
+    </row>
+    <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:J31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="11.54296875" style="63" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="63"/>
+    <col min="9" max="16384" width="11.54296875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="66" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +1811,7 @@
       <c r="E4" s="66"/>
       <c r="F4" s="66"/>
     </row>
-    <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="63" t="s">
         <v>19</v>
       </c>
@@ -1448,22 +1819,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="63" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="63" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="63" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="63" t="s">
         <v>1</v>
       </c>
@@ -1480,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="63">
         <v>1</v>
       </c>
@@ -1495,7 +1866,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="63">
         <v>2</v>
       </c>
@@ -1509,7 +1880,7 @@
         <v>499.99</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="63">
         <v>3</v>
       </c>
@@ -1523,7 +1894,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="63">
         <v>4</v>
       </c>
@@ -1537,7 +1908,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="63">
         <v>5</v>
       </c>
@@ -1555,7 +1926,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="63">
         <v>6</v>
       </c>
@@ -1572,7 +1943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="63">
         <v>7</v>
       </c>
@@ -1589,7 +1960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="63">
         <v>8</v>
       </c>
@@ -1606,7 +1977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="63">
         <v>9</v>
       </c>
@@ -1623,7 +1994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="63">
         <v>10</v>
       </c>
@@ -1640,12 +2011,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="63" t="s">
         <v>14</v>
       </c>
@@ -1653,12 +2024,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="63" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="63" t="s">
         <v>15</v>
       </c>
@@ -1666,7 +2037,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="63" t="s">
         <v>16</v>
       </c>
@@ -1675,7 +2046,7 @@
       </c>
       <c r="F29" s="64"/>
     </row>
-    <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="63" t="s">
         <v>17</v>
       </c>
@@ -1685,34 +2056,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="2.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="33.26953125" style="3" customWidth="1"/>
     <col min="4" max="4" width="100" style="3" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="1.7265625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="76" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="76"/>
       <c r="D2" s="76"/>
     </row>
-    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" s="77" t="s">
         <v>26</v>
       </c>
@@ -1720,34 +2091,34 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="77"/>
       <c r="D5" s="69" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" s="77"/>
       <c r="D6" s="70" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" s="77"/>
       <c r="D7" s="69" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="77"/>
       <c r="D8" s="71" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="67"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="77" t="s">
         <v>32</v>
       </c>
@@ -1755,13 +2126,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11" s="77"/>
       <c r="D11" s="73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="77"/>
       <c r="D12" s="74" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
mise en page "identification du client"
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF422200-DE73-48A5-994C-8E26E721F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D2D846-556D-4DF0-A4BE-52C7710116F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,7 +155,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +311,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -386,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -516,12 +523,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,6 +815,27 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1501,7 +1547,7 @@
   <dimension ref="A2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1535,27 +1581,46 @@
       <c r="F4" s="80"/>
     </row>
     <row r="6" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="63" t="s">
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="83" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="83"/>
+      <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="63" t="s">
+      <c r="A7" s="84"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85" t="s">
         <v>22</v>
       </c>
+      <c r="E7" s="85"/>
+      <c r="F7" s="84"/>
     </row>
     <row r="8" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="63" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85" t="s">
         <v>21</v>
       </c>
+      <c r="E8" s="85"/>
+      <c r="F8" s="84"/>
     </row>
     <row r="9" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="63" t="s">
+      <c r="A9" s="86"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="87" t="s">
         <v>23</v>
       </c>
+      <c r="E9" s="87"/>
+      <c r="F9" s="86"/>
     </row>
     <row r="11" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="63" t="s">

</xml_diff>

<commit_message>
total fait et mis en dollar
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D2D846-556D-4DF0-A4BE-52C7710116F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D21CD0-9D87-48B2-BC6E-2B2768B2487F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -546,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +836,15 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1547,7 +1556,7 @@
   <dimension ref="A2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D12" sqref="D12:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1646,11 +1655,15 @@
       <c r="C12" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="90">
         <v>15</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="88">
         <v>45</v>
+      </c>
+      <c r="F12" s="89">
+        <f>D12*E12</f>
+        <v>675</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -1661,11 +1674,15 @@
       <c r="C13" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="90">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="88">
         <v>499.99</v>
+      </c>
+      <c r="F13" s="89">
+        <f t="shared" ref="F13:F15" si="0">D13*E13</f>
+        <v>999.98</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1675,11 +1692,15 @@
       <c r="C14" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="90">
         <v>5</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="88">
         <v>45</v>
+      </c>
+      <c r="F14" s="89">
+        <f t="shared" si="0"/>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,11 +1710,15 @@
       <c r="C15" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="90">
         <v>120</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="88">
         <v>85</v>
+      </c>
+      <c r="F15" s="89">
+        <f t="shared" si="0"/>
+        <v>10200</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mise en page du tableau de données
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D21CD0-9D87-48B2-BC6E-2B2768B2487F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42326DE-8AAA-4D69-A7E1-9F08D2F8B12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="36">
   <si>
     <t>Compagnie X</t>
   </si>
@@ -155,7 +155,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,8 +318,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +397,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -837,14 +851,47 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1553,24 +1600,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6281C5BB-372A-4902-85E9-DFBE7E384DD1}">
-  <dimension ref="A2:J31"/>
+  <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D15"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" style="63" customWidth="1"/>
+    <col min="1" max="1" width="2.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.54296875" style="63" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" style="63" customWidth="1"/>
+    <col min="3" max="3" width="47.08984375" style="63" customWidth="1"/>
     <col min="4" max="7" width="11.54296875" style="63" customWidth="1"/>
     <col min="8" max="8" width="11.54296875" style="63"/>
     <col min="9" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="78"/>
+    <row r="2" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="78" t="s">
         <v>0</v>
       </c>
@@ -1579,18 +1625,14 @@
       <c r="E2" s="79"/>
       <c r="F2" s="79"/>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="80" t="s">
-        <v>18</v>
-      </c>
+    <row r="4" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
       <c r="F4" s="80"/>
     </row>
-    <row r="6" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
+    <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="81"/>
       <c r="C6" s="82" t="s">
         <v>19</v>
@@ -1601,8 +1643,7 @@
       <c r="E6" s="83"/>
       <c r="F6" s="81"/>
     </row>
-    <row r="7" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
+    <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="84"/>
       <c r="C7" s="84"/>
       <c r="D7" s="85" t="s">
@@ -1611,8 +1652,7 @@
       <c r="E7" s="85"/>
       <c r="F7" s="84"/>
     </row>
-    <row r="8" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
+    <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="84"/>
       <c r="C8" s="84"/>
       <c r="D8" s="85" t="s">
@@ -1621,8 +1661,7 @@
       <c r="E8" s="85"/>
       <c r="F8" s="84"/>
     </row>
-    <row r="9" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
+    <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="86"/>
       <c r="C9" s="86"/>
       <c r="D9" s="87" t="s">
@@ -1631,53 +1670,53 @@
       <c r="E9" s="87"/>
       <c r="F9" s="86"/>
     </row>
-    <row r="11" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="63" t="s">
+    <row r="11" spans="2:10" ht="11.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="90" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="63">
+    <row r="12" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="91">
         <v>1</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="90">
+      <c r="D12" s="92">
         <v>15</v>
       </c>
       <c r="E12" s="88">
         <v>45</v>
       </c>
-      <c r="F12" s="89">
+      <c r="F12" s="88">
         <f>D12*E12</f>
         <v>675</v>
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="63">
+    <row r="13" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="93">
         <v>2</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="90">
+      <c r="D13" s="95">
         <v>2</v>
       </c>
-      <c r="E13" s="88">
+      <c r="E13" s="89">
         <v>499.99</v>
       </c>
       <c r="F13" s="89">
@@ -1685,35 +1724,35 @@
         <v>999.98</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="63">
+    <row r="14" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="91">
         <v>3</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="90">
+      <c r="D14" s="92">
         <v>5</v>
       </c>
       <c r="E14" s="88">
         <v>45</v>
       </c>
-      <c r="F14" s="89">
+      <c r="F14" s="88">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="63">
+    <row r="15" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="93">
         <v>4</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="90">
+      <c r="D15" s="95">
         <v>120</v>
       </c>
-      <c r="E15" s="88">
+      <c r="E15" s="89">
         <v>85</v>
       </c>
       <c r="F15" s="89">
@@ -1721,106 +1760,106 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="63">
+    <row r="16" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="96">
         <v>5</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="D16" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="65" t="s">
+      <c r="E16" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="97" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="63">
+      <c r="B17" s="98">
         <v>6</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="65" t="s">
+      <c r="E17" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="99" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="63">
+      <c r="B18" s="96">
         <v>7</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="65" t="s">
+      <c r="E18" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="97" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="63">
-        <v>8</v>
-      </c>
-      <c r="C19" s="65" t="s">
+      <c r="B19" s="98">
+        <v>8</v>
+      </c>
+      <c r="C19" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="65" t="s">
+      <c r="E19" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="99" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="63">
+      <c r="B20" s="96">
         <v>9</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="65" t="s">
+      <c r="E20" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="97" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="63">
+      <c r="B21" s="100">
         <v>10</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="65" t="s">
+      <c r="E21" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="101" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1866,7 +1905,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
calcul des totaux dans la tableau de total
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42326DE-8AAA-4D69-A7E1-9F08D2F8B12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62950014-92B8-43B0-A714-76A63BBE87BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
@@ -556,11 +557,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,10 +895,23 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1603,7 +1618,7 @@
   <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1867,6 +1882,10 @@
       <c r="D23" s="63" t="s">
         <v>13</v>
       </c>
+      <c r="F23" s="102">
+        <f>SUM(F12:F15)</f>
+        <v>12099.98</v>
+      </c>
     </row>
     <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="63" t="s">
@@ -1880,13 +1899,21 @@
       <c r="D26" s="63" t="s">
         <v>13</v>
       </c>
+      <c r="F26" s="103">
+        <f>F23-F25</f>
+        <v>11599.98</v>
+      </c>
     </row>
     <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="104">
         <v>0.05</v>
+      </c>
+      <c r="F28" s="103">
+        <f>F26*E28</f>
+        <v>579.99900000000002</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1896,11 +1923,18 @@
       <c r="E29" s="63">
         <v>9.9750000000000005E-2</v>
       </c>
-      <c r="F29" s="64"/>
+      <c r="F29" s="105">
+        <f>F26*E29</f>
+        <v>1157.0980050000001</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="63" t="s">
         <v>17</v>
+      </c>
+      <c r="F31" s="103">
+        <f>SUM(F26:F29)</f>
+        <v>13337.077004999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en page du tableau de total
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62950014-92B8-43B0-A714-76A63BBE87BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183E5F7B-E964-4DED-AA1E-B9D562ADC09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,8 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
@@ -562,7 +561,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -853,6 +852,9 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -895,16 +897,43 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1618,7 +1647,7 @@
   <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1686,253 +1715,269 @@
       <c r="F9" s="86"/>
     </row>
     <row r="11" spans="2:10" ht="11.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="90" t="s">
+      <c r="E11" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="90" t="s">
+      <c r="F11" s="91" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="91">
+      <c r="B12" s="92">
         <v>1</v>
       </c>
       <c r="C12" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="92">
+      <c r="D12" s="93">
         <v>15</v>
       </c>
-      <c r="E12" s="88">
+      <c r="E12" s="89">
         <v>45</v>
       </c>
-      <c r="F12" s="88">
+      <c r="F12" s="89">
         <f>D12*E12</f>
         <v>675</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="93">
+      <c r="B13" s="94">
         <v>2</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="96">
         <v>2</v>
       </c>
-      <c r="E13" s="89">
+      <c r="E13" s="90">
         <v>499.99</v>
       </c>
-      <c r="F13" s="89">
+      <c r="F13" s="90">
         <f t="shared" ref="F13:F15" si="0">D13*E13</f>
         <v>999.98</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="91">
+      <c r="B14" s="92">
         <v>3</v>
       </c>
       <c r="C14" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="92">
+      <c r="D14" s="93">
         <v>5</v>
       </c>
-      <c r="E14" s="88">
+      <c r="E14" s="89">
         <v>45</v>
       </c>
-      <c r="F14" s="88">
+      <c r="F14" s="89">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="93">
+      <c r="B15" s="94">
         <v>4</v>
       </c>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="95">
+      <c r="D15" s="96">
         <v>120</v>
       </c>
-      <c r="E15" s="89">
+      <c r="E15" s="90">
         <v>85</v>
       </c>
-      <c r="F15" s="89">
+      <c r="F15" s="90">
         <f t="shared" si="0"/>
         <v>10200</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="96">
+      <c r="B16" s="97">
         <v>5</v>
       </c>
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="D16" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="97" t="s">
+      <c r="E16" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="98" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="98">
+      <c r="B17" s="99">
         <v>6</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="99" t="s">
+      <c r="E17" s="100" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="100" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="96">
+      <c r="B18" s="97">
         <v>7</v>
       </c>
-      <c r="C18" s="97" t="s">
+      <c r="C18" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="97" t="s">
+      <c r="D18" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="97" t="s">
+      <c r="E18" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="98" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="98">
-        <v>8</v>
-      </c>
-      <c r="C19" s="99" t="s">
+      <c r="B19" s="99">
+        <v>8</v>
+      </c>
+      <c r="C19" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="99" t="s">
+      <c r="E19" s="100" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="100" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="96">
+      <c r="B20" s="97">
         <v>9</v>
       </c>
-      <c r="C20" s="97" t="s">
+      <c r="C20" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="97" t="s">
+      <c r="D20" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="97" t="s">
+      <c r="E20" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="98" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="100">
+      <c r="B21" s="101">
         <v>10</v>
       </c>
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="101" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="101" t="s">
+      <c r="E21" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="102" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="102">
+      <c r="E23" s="105"/>
+      <c r="F23" s="106">
         <f>SUM(F12:F15)</f>
         <v>12099.98</v>
       </c>
     </row>
+    <row r="24" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="103"/>
+      <c r="F24" s="88"/>
+    </row>
     <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="63" t="s">
+      <c r="D25" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="64">
+      <c r="E25" s="108"/>
+      <c r="F25" s="109">
         <v>500</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="63" t="s">
+      <c r="D26" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="103">
+      <c r="E26" s="111"/>
+      <c r="F26" s="112">
         <f>F23-F25</f>
         <v>11599.98</v>
       </c>
     </row>
+    <row r="27" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="103"/>
+      <c r="F27" s="88"/>
+    </row>
     <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="63" t="s">
+      <c r="D28" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="104">
+      <c r="E28" s="113">
         <v>0.05</v>
       </c>
-      <c r="F28" s="103">
+      <c r="F28" s="109">
         <f>F26*E28</f>
         <v>579.99900000000002</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="63" t="s">
+      <c r="D29" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="63">
+      <c r="E29" s="114">
         <v>9.9750000000000005E-2</v>
       </c>
-      <c r="F29" s="105">
+      <c r="F29" s="112">
         <f>F26*E29</f>
         <v>1157.0980050000001</v>
       </c>
     </row>
+    <row r="30" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="103"/>
+      <c r="F30" s="88"/>
+    </row>
     <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="103">
+      <c r="E31" s="105"/>
+      <c r="F31" s="115">
         <f>SUM(F26:F29)</f>
         <v>13337.077004999999</v>
       </c>

</xml_diff>

<commit_message>
Modification d'un sous titre
Ajout du terme :  Facture  -  W458
</commit_message>
<xml_diff>
--- a/Excel_Exercice02_FormulesEtOperateurs.xlsx
+++ b/Excel_Exercice02_FormulesEtOperateurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183E5F7B-E964-4DED-AA1E-B9D562ADC09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF9C445-2B48-4C40-80B8-F74C2BF24ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
   <si>
     <t>Compagnie X</t>
   </si>
@@ -810,10 +810,124 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -821,120 +935,6 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1311,13 +1311,13 @@
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
@@ -1647,7 +1647,7 @@
   <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1661,323 +1661,325 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
     </row>
     <row r="4" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+      <c r="B4" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
     </row>
     <row r="6" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
-      <c r="C6" s="82" t="s">
+      <c r="B6" s="77"/>
+      <c r="C6" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="81"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="77"/>
     </row>
     <row r="7" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="85" t="s">
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="84"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="80"/>
     </row>
     <row r="8" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="85" t="s">
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="85"/>
-      <c r="F8" s="84"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="80"/>
     </row>
     <row r="9" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="87" t="s">
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="86"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="82"/>
     </row>
     <row r="11" spans="2:10" ht="11.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="F11" s="87" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="92">
+      <c r="B12" s="88">
         <v>1</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="93">
+      <c r="D12" s="89">
         <v>15</v>
       </c>
-      <c r="E12" s="89">
+      <c r="E12" s="85">
         <v>45</v>
       </c>
-      <c r="F12" s="89">
+      <c r="F12" s="85">
         <f>D12*E12</f>
         <v>675</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="94">
+      <c r="B13" s="90">
         <v>2</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="92">
         <v>2</v>
       </c>
-      <c r="E13" s="90">
+      <c r="E13" s="86">
         <v>499.99</v>
       </c>
-      <c r="F13" s="90">
+      <c r="F13" s="86">
         <f t="shared" ref="F13:F15" si="0">D13*E13</f>
         <v>999.98</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="92">
+      <c r="B14" s="88">
         <v>3</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="93">
+      <c r="D14" s="89">
         <v>5</v>
       </c>
-      <c r="E14" s="89">
+      <c r="E14" s="85">
         <v>45</v>
       </c>
-      <c r="F14" s="89">
+      <c r="F14" s="85">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="94">
+      <c r="B15" s="90">
         <v>4</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="96">
+      <c r="D15" s="92">
         <v>120</v>
       </c>
-      <c r="E15" s="90">
+      <c r="E15" s="86">
         <v>85</v>
       </c>
-      <c r="F15" s="90">
+      <c r="F15" s="86">
         <f t="shared" si="0"/>
         <v>10200</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="97">
+      <c r="B16" s="93">
         <v>5</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="98" t="s">
+      <c r="E16" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="94" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="99">
+      <c r="B17" s="95">
         <v>6</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="100" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="100" t="s">
+      <c r="E17" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="96" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="97">
+      <c r="B18" s="93">
         <v>7</v>
       </c>
-      <c r="C18" s="98" t="s">
+      <c r="C18" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="98" t="s">
+      <c r="E18" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="99">
-        <v>8</v>
-      </c>
-      <c r="C19" s="100" t="s">
+      <c r="B19" s="95">
+        <v>8</v>
+      </c>
+      <c r="C19" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="100" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="100" t="s">
+      <c r="E19" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="96" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97">
+      <c r="B20" s="93">
         <v>9</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="98" t="s">
+      <c r="E20" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="94" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="101">
+      <c r="B21" s="97">
         <v>10</v>
       </c>
-      <c r="C21" s="102" t="s">
+      <c r="C21" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="102" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="102" t="s">
+      <c r="E21" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="98" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="104" t="s">
+      <c r="D23" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="105"/>
-      <c r="F23" s="106">
+      <c r="E23" s="101"/>
+      <c r="F23" s="102">
         <f>SUM(F12:F15)</f>
         <v>12099.98</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="103"/>
-      <c r="F24" s="88"/>
+      <c r="D24" s="99"/>
+      <c r="F24" s="84"/>
     </row>
     <row r="25" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="107" t="s">
+      <c r="D25" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="108"/>
-      <c r="F25" s="109">
+      <c r="E25" s="104"/>
+      <c r="F25" s="105">
         <v>500</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="110" t="s">
+      <c r="D26" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="112">
+      <c r="E26" s="107"/>
+      <c r="F26" s="108">
         <f>F23-F25</f>
         <v>11599.98</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="103"/>
-      <c r="F27" s="88"/>
+      <c r="D27" s="99"/>
+      <c r="F27" s="84"/>
     </row>
     <row r="28" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="107" t="s">
+      <c r="D28" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="113">
+      <c r="E28" s="109">
         <v>0.05</v>
       </c>
-      <c r="F28" s="109">
+      <c r="F28" s="105">
         <f>F26*E28</f>
         <v>579.99900000000002</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="110" t="s">
+      <c r="D29" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="114">
+      <c r="E29" s="110">
         <v>9.9750000000000005E-2</v>
       </c>
-      <c r="F29" s="112">
+      <c r="F29" s="108">
         <f>F26*E29</f>
         <v>1157.0980050000001</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="103"/>
-      <c r="F30" s="88"/>
+      <c r="D30" s="99"/>
+      <c r="F30" s="84"/>
     </row>
     <row r="31" spans="2:6" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="104" t="s">
+      <c r="D31" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="105"/>
-      <c r="F31" s="115">
+      <c r="E31" s="101"/>
+      <c r="F31" s="111">
         <f>SUM(F26:F29)</f>
         <v>13337.077004999999</v>
       </c>
@@ -1995,7 +1997,7 @@
   <dimension ref="A2:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2284,15 +2286,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="115" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="68" t="s">
@@ -2300,25 +2302,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="77"/>
+      <c r="C5" s="115"/>
       <c r="D5" s="69" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="77"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="70" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="77"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="69" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="77"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="71" t="s">
         <v>31</v>
       </c>
@@ -2327,7 +2329,7 @@
       <c r="C9" s="67"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="115" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="72" t="s">
@@ -2335,13 +2337,13 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="77"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="73" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="77"/>
+      <c r="C12" s="115"/>
       <c r="D12" s="74" t="s">
         <v>34</v>
       </c>

</xml_diff>